<commit_message>
Build Your First Process With Studio Complete
</commit_message>
<xml_diff>
--- a/Email Automation/Invoices/Invoice 2.xlsx
+++ b/Email Automation/Invoices/Invoice 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denni\Documents\UiPath\Email Automation\Invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961C6518-C000-4E91-BD22-1A632B6F2087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D966B2B-86A3-4EC1-A87E-E2C17E9FE645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="0" windowWidth="14580" windowHeight="15480" xr2:uid="{ACCB1FA6-7E67-4590-BB25-A17FCE65C786}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>BILL TO</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>CLIENT CODE</t>
-  </si>
-  <si>
-    <t>This client doesn't benefit from any discount</t>
   </si>
   <si>
     <t>RPA Dev, developer.rpa@mail.com</t>
@@ -1189,12 +1186,12 @@
       <c r="D18" s="34">
         <v>1</v>
       </c>
-      <c r="E18" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="36" t="e">
+      <c r="E18" s="35">
+        <v>0</v>
+      </c>
+      <c r="F18" s="36">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1229,9 +1226,9 @@
         <v>13</v>
       </c>
       <c r="E21" s="48"/>
-      <c r="F21" s="22" t="e">
+      <c r="F21" s="22">
         <f>SUM(F16:F20)</f>
-        <v>#VALUE!</v>
+        <v>950</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1254,9 +1251,9 @@
         <v>15</v>
       </c>
       <c r="E23" s="16"/>
-      <c r="F23" s="12" t="e">
+      <c r="F23" s="12">
         <f>F21*F22</f>
-        <v>#VALUE!</v>
+        <v>40.375</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -1267,9 +1264,9 @@
         <v>16</v>
       </c>
       <c r="E24" s="52"/>
-      <c r="F24" s="17" t="e">
+      <c r="F24" s="17">
         <f>F21+F23</f>
-        <v>#VALUE!</v>
+        <v>990.375</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1322,7 +1319,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>

</xml_diff>